<commit_message>
Rimossi file .txt della configurazione slides
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/SourceFiles/DataSource.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/SourceFiles/DataSource.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="851" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Superdettagli" sheetId="1" r:id="rId1"/>
@@ -7400,7 +7400,7 @@
   <dimension ref="A1:Z93"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8309,8 +8309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9385,7 +9385,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9898,8 +9898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Codice posizionamento immagine nel box
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/SourceFiles/DataSource.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/SourceFiles/DataSource.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="774" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16215" tabRatio="774" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="3" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="275">
   <si>
     <t>da considerare?_</t>
   </si>
@@ -820,12 +820,6 @@
     <t>Progetti U (produttive indirette)</t>
   </si>
   <si>
-    <t>Progetti per business</t>
-  </si>
-  <si>
-    <t>Progetti per projectType</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -897,9 +891,6 @@
     <t>Presentazione casi test.pptx</t>
   </si>
   <si>
-    <t>C1:P39</t>
-  </si>
-  <si>
     <t>D1:P30</t>
   </si>
   <si>
@@ -910,6 +901,24 @@
   </si>
   <si>
     <t>PP_17</t>
+  </si>
+  <si>
+    <t>Una slide</t>
+  </si>
+  <si>
+    <t>2 slides verticali</t>
+  </si>
+  <si>
+    <t>2 slides orizzontali</t>
+  </si>
+  <si>
+    <t>3 slides verticali</t>
+  </si>
+  <si>
+    <t>3 slides orizzontali</t>
+  </si>
+  <si>
+    <t>D1:P39</t>
   </si>
 </sst>
 </file>
@@ -4830,8 +4839,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="388716904"/>
-        <c:axId val="388718472"/>
+        <c:axId val="166125680"/>
+        <c:axId val="388007984"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5131,11 +5140,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="388716904"/>
-        <c:axId val="388718472"/>
+        <c:axId val="166125680"/>
+        <c:axId val="388007984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="388716904"/>
+        <c:axId val="166125680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5178,7 +5187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388718472"/>
+        <c:crossAx val="388007984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5186,7 +5195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="388718472"/>
+        <c:axId val="388007984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5238,7 +5247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388716904"/>
+        <c:crossAx val="166125680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5926,8 +5935,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9162143" y="965201"/>
-          <a:ext cx="1151488" cy="751113"/>
+          <a:off x="8768443" y="962026"/>
+          <a:ext cx="1151488" cy="741588"/>
           <a:chOff x="1230086" y="4294415"/>
           <a:chExt cx="1151488" cy="713013"/>
         </a:xfrm>
@@ -6163,8 +6172,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9183919" y="2189843"/>
-          <a:ext cx="1126672" cy="796471"/>
+          <a:off x="8790219" y="2167618"/>
+          <a:ext cx="1126672" cy="783771"/>
           <a:chOff x="1230090" y="5464629"/>
           <a:chExt cx="1126672" cy="745671"/>
         </a:xfrm>
@@ -7257,55 +7266,55 @@
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="131" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B1" s="132"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="91" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="89" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="85"/>
       <c r="B5" s="86" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="85" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B6" s="86"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B7" s="86" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7389,43 +7398,43 @@
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="131" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B1" s="132"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="91" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="85" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5" s="86" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7539,7 +7548,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="84" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="60"/>
@@ -8033,7 +8042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -8068,7 +8077,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C2" s="116"/>
       <c r="D2" s="60"/>
@@ -9188,7 +9197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -9259,7 +9268,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" s="93" t="str">
         <f>D1</f>
@@ -10926,7 +10935,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -12593,7 +12602,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -14260,7 +14269,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -15927,7 +15936,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -17594,7 +17603,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -19590,7 +19599,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -21257,7 +21266,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -22924,7 +22933,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -24591,7 +24600,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -26258,7 +26267,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -27925,7 +27934,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -29592,7 +29601,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -31203,7 +31212,7 @@
       </c>
       <c r="B1" s="139"/>
       <c r="D1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E1" t="str">
         <f>D1</f>
@@ -31259,7 +31268,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -32870,7 +32879,7 @@
       </c>
       <c r="B1" s="139"/>
       <c r="D1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E1" t="str">
         <f>D1</f>
@@ -32926,7 +32935,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -34537,7 +34546,7 @@
       </c>
       <c r="B1" s="139"/>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E1" t="str">
         <f>D1</f>
@@ -34593,7 +34602,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f>D1</f>
@@ -37497,282 +37506,282 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -38209,2882 +38218,2882 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B41" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B42" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B44" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B45" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B47" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B48" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B51" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B52" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B53" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B55" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B56" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B57" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B58" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B61" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B62" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B66" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B68" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B82" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B84" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B89" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B92" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B93" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B94" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B96" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B97" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B98" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B100" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B102" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B103" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B105" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B106" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B107" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B108" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B109" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B110" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B111" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B112" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B113" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B114" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B115" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B116" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B119" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B120" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B121" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B126" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B127" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B129" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B131" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B133" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B136" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B137" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B138" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B139" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B141" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B142" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B143" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B144" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B145" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B146" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B147" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B148" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B149" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B150" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B151" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B152" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B153" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B154" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B155" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B156" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B157" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B158" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B159" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B160" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B161" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B162" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B163" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B164" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B165" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B166" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B167" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B168" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B169" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B170" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B171" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B172" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B173" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B174" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B175" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B176" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B177" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B178" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B179" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B180" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B181" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B182" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B183" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B184" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B185" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B186" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B187" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B188" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B189" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B190" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B191" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B192" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B193" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B194" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B195" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B196" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B197" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B198" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B199" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B200" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B201" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B202" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B203" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B204" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B205" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B206" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B207" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B208" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B209" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B210" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B211" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B212" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B213" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B214" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B215" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B216" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B217" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B218" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B219" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B220" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B221" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B222" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B223" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B224" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B225" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B226" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B227" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B228" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B229" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B230" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B231" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B232" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B233" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B234" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B235" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B237" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B238" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B239" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B240" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B242" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B243" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B244" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B245" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B248" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B249" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B250" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B251" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B252" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B253" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B254" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B255" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B256" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B257" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B258" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B259" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B260" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B261" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B262" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B263" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B264" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B265" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B266" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B267" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B268" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B269" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B270" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B271" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B272" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B273" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B274" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B275" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B276" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B277" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B278" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B279" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B280" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B281" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B282" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B283" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B284" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B285" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B286" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B287" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B288" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B289" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B290" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B291" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B292" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B293" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B294" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B295" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B296" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B297" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B298" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B299" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B300" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B301" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B302" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B303" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B304" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B305" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B306" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B307" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B308" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B309" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B310" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B311" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B312" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B313" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B314" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B315" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B316" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B317" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B318" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B319" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B320" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B321" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B322" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B323" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B324" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B325" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B326" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B327" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B328" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B329" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B330" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B331" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B332" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B333" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B334" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B335" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B336" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B337" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B338" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B339" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B340" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B341" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B342" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B343" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B344" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B345" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B346" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B347" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B348" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B349" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B350" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B351" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B352" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B353" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B354" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B355" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B356" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B357" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B358" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B359" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B360" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B361" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B362" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B363" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -41103,7 +41112,7 @@
   <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41154,7 +41163,7 @@
         <v>206</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C3" s="69" t="s">
         <v>207</v>
@@ -41498,10 +41507,10 @@
     </row>
     <row r="18" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="C18" s="94" t="s">
         <v>185</v>
@@ -41519,16 +41528,16 @@
     </row>
     <row r="19" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="95" t="s">
@@ -41544,16 +41553,16 @@
     </row>
     <row r="20" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E20" s="69"/>
       <c r="F20" s="95" t="s">
@@ -41569,19 +41578,19 @@
     </row>
     <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B21" t="s">
-        <v>231</v>
+        <v>272</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D21" s="69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E21" s="69" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F21" s="95" t="s">
         <v>211</v>
@@ -41594,21 +41603,21 @@
       <c r="L21" s="66"/>
       <c r="M21" s="66"/>
     </row>
-    <row r="22" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D22" s="69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E22" s="69" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F22" s="95" t="s">
         <v>199</v>
@@ -41622,18 +41631,12 @@
       <c r="M22" s="66"/>
     </row>
     <row r="23" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>266</v>
-      </c>
-      <c r="B23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C23" s="69" t="s">
-        <v>191</v>
-      </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="95"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
       <c r="G23" s="66"/>
       <c r="H23" s="66"/>
       <c r="I23" s="66"/>
@@ -41642,19 +41645,11 @@
       <c r="L23" s="66"/>
       <c r="M23" s="66"/>
     </row>
-    <row r="24" spans="1:13" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="60" t="s">
-        <v>266</v>
-      </c>
-      <c r="B24" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="C24" s="96" t="s">
-        <v>192</v>
-      </c>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="97"/>
+    <row r="24" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="69"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
       <c r="G24" s="66"/>
       <c r="H24" s="66"/>
       <c r="I24" s="66"/>
@@ -41664,12 +41659,10 @@
       <c r="M24" s="66"/>
     </row>
     <row r="25" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="66"/>
       <c r="H25" s="66"/>
       <c r="I25" s="66"/>

</xml_diff>